<commit_message>
Update FRATAR regression coefficients
</commit_message>
<xml_diff>
--- a/Parameter/FLUAM_ControlFile.xlsx
+++ b/Parameter/FLUAM_ControlFile.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Models\StateWide\TSM_Legacy\workdir\FLUAM\Process15_20\R8\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Models\StateWide\TSM_Legacy\FLUAM\Parameter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF3C6D2F-F9F5-4897-BB2F-DAC196B712F1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F595D1E4-CD25-47FF-ACCA-F9A384B5E78B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0BE306DF-5F1F-4431-8911-019B31789681}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0BE306DF-5F1F-4431-8911-019B31789681}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,34 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="155">
-  <si>
-    <t>LOAD_BIGDUMP.TXT</t>
-  </si>
-  <si>
-    <t>d_TAZ_2015_In.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Growth_15to20.csv   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">d_Nodes.txt        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">d_Links.txt     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DensityConstraints.csv </t>
-  </si>
-  <si>
-    <t>d_TAZ_Out.csv</t>
-  </si>
-  <si>
-    <t>d_TAZ_Next_In.csv</t>
-  </si>
-  <si>
-    <t>d_FratarInput.txt</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="133">
   <si>
     <t>Value</t>
   </si>
@@ -108,45 +81,12 @@
     <t>TRANEMP (Area Type 3)</t>
   </si>
   <si>
-    <t>WGHT_HH</t>
-  </si>
-  <si>
     <t>Urban area</t>
   </si>
   <si>
-    <t>INPUT: travel time skim</t>
-  </si>
-  <si>
-    <t>INPUT: TAZ input file for LUAM</t>
-  </si>
-  <si>
-    <t>INPUT: growth file</t>
-  </si>
-  <si>
-    <t>INPUT: node file</t>
-  </si>
-  <si>
-    <t>INPUT: link file</t>
-  </si>
-  <si>
-    <t>INPUT: density constraints file</t>
-  </si>
-  <si>
-    <t>OUTPUT: zonal outupt file</t>
-  </si>
-  <si>
-    <t>OUTPUT: zonal output file to be used as next input TAZ file</t>
-  </si>
-  <si>
-    <t>Files</t>
-  </si>
-  <si>
     <t>constant</t>
   </si>
   <si>
-    <t>if outside the urban growth boundry</t>
-  </si>
-  <si>
     <t>distance to coast (dis_coast)</t>
   </si>
   <si>
@@ -285,33 +225,6 @@
     <t>ctl.7</t>
   </si>
   <si>
-    <t>F.1</t>
-  </si>
-  <si>
-    <t>F.2</t>
-  </si>
-  <si>
-    <t>F.3</t>
-  </si>
-  <si>
-    <t>F.4</t>
-  </si>
-  <si>
-    <t>F.5</t>
-  </si>
-  <si>
-    <t>F.6</t>
-  </si>
-  <si>
-    <t>F.7</t>
-  </si>
-  <si>
-    <t>F.8</t>
-  </si>
-  <si>
-    <t>F.9</t>
-  </si>
-  <si>
     <t>Key</t>
   </si>
   <si>
@@ -496,13 +409,37 @@
   </si>
   <si>
     <t>fratUrbanArea</t>
+  </si>
+  <si>
+    <t>fratHHFact.1</t>
+  </si>
+  <si>
+    <t>RURHH (Area Type 1)</t>
+  </si>
+  <si>
+    <t>fratHHFact.2</t>
+  </si>
+  <si>
+    <t>URBHH (Area Type 2)</t>
+  </si>
+  <si>
+    <t>fratHHFact.3</t>
+  </si>
+  <si>
+    <t>TRANHH (Area Type 3)</t>
+  </si>
+  <si>
+    <t>if inside the urban growth boundry</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -526,20 +463,44 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Courier"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
+      <name val="Courier"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -547,17 +508,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 3 2 2" xfId="1" xr:uid="{A203302A-CD45-4B15-9C1D-D835CD5327B8}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -872,1051 +853,1051 @@
   <dimension ref="A1:D74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="54.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>93</v>
+        <v>64</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="5">
+        <v>0</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="5">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="5">
+        <v>6424</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="5">
+        <v>6461</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="5">
+        <v>100</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C5">
-        <v>6424</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C6">
-        <v>6461</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C7">
-        <v>100</v>
-      </c>
-      <c r="D7" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="C8">
         <v>-1.7354000000000001</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>148</v>
-      </c>
-      <c r="C9">
-        <v>1147.7840000000001</v>
+        <v>119</v>
+      </c>
+      <c r="C9" s="2">
+        <v>565.88554648212198</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>149</v>
+        <v>120</v>
       </c>
       <c r="B10" t="s">
-        <v>150</v>
-      </c>
-      <c r="C10">
-        <v>3.61</v>
+        <v>121</v>
+      </c>
+      <c r="C10" s="3">
+        <v>10.809144997514515</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>149</v>
+        <v>120</v>
       </c>
       <c r="B11" t="s">
-        <v>151</v>
-      </c>
-      <c r="C11">
-        <v>3.024</v>
+        <v>122</v>
+      </c>
+      <c r="C11" s="3">
+        <v>7.0701320225179662</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>149</v>
+        <v>120</v>
       </c>
       <c r="B12" t="s">
-        <v>152</v>
-      </c>
-      <c r="C12">
-        <v>3.952</v>
+        <v>123</v>
+      </c>
+      <c r="C12" s="3">
+        <v>10.048530361121582</v>
       </c>
       <c r="D12" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" t="s">
-        <v>153</v>
-      </c>
-      <c r="C13">
-        <v>1.8839999999999999</v>
+      <c r="A13" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C13" s="2">
+        <v>4.2834951692240191</v>
       </c>
       <c r="D13" t="s">
-        <v>25</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" t="s">
-        <v>154</v>
-      </c>
-      <c r="C14">
-        <v>1611.567</v>
+      <c r="A14" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C14" s="2">
+        <v>10.149223712027361</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" t="s">
-        <v>84</v>
-      </c>
-      <c r="C15" t="s">
-        <v>0</v>
+      <c r="A15" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C15" s="2">
+        <v>6.4854738028603665</v>
       </c>
       <c r="D15" t="s">
-        <v>27</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>85</v>
-      </c>
-      <c r="C16" t="s">
-        <v>1</v>
+        <v>125</v>
+      </c>
+      <c r="C16" s="2">
+        <v>955.26841206494112</v>
       </c>
       <c r="D16" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>86</v>
-      </c>
-      <c r="C17" t="s">
-        <v>2</v>
+        <v>65</v>
+      </c>
+      <c r="C17">
+        <v>-0.7</v>
       </c>
       <c r="D17" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B18" t="s">
-        <v>87</v>
-      </c>
-      <c r="C18" t="s">
-        <v>3</v>
+        <v>66</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>30</v>
+        <v>132</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B19" t="s">
-        <v>88</v>
-      </c>
-      <c r="C19" t="s">
-        <v>4</v>
+        <v>67</v>
+      </c>
+      <c r="C19">
+        <v>-2.7230000000000002E-3</v>
       </c>
       <c r="D19" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B20" t="s">
-        <v>89</v>
-      </c>
-      <c r="C20" t="s">
-        <v>5</v>
+        <v>68</v>
+      </c>
+      <c r="C20">
+        <v>2.4</v>
       </c>
       <c r="D20" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B21" t="s">
-        <v>90</v>
-      </c>
-      <c r="C21" t="s">
-        <v>6</v>
+        <v>69</v>
+      </c>
+      <c r="C21">
+        <v>-0.2</v>
       </c>
       <c r="D21" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B22" t="s">
-        <v>91</v>
-      </c>
-      <c r="C22" t="s">
-        <v>7</v>
+        <v>70</v>
+      </c>
+      <c r="C22">
+        <v>0.18</v>
       </c>
       <c r="D22" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B23" t="s">
-        <v>92</v>
-      </c>
-      <c r="C23" t="s">
-        <v>8</v>
+        <v>72</v>
+      </c>
+      <c r="C23">
+        <v>-0.75</v>
       </c>
       <c r="D23" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="B24" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="C24">
-        <v>-0.7</v>
+        <v>1.23</v>
       </c>
       <c r="D24" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="B25" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="C25">
-        <v>4</v>
+        <v>-0.77</v>
       </c>
       <c r="D25" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="C26">
-        <v>-2.7230000000000002E-3</v>
+        <v>-0.97</v>
       </c>
       <c r="D26" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="B27" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="C27">
-        <v>2.4</v>
+        <v>0</v>
       </c>
       <c r="D27" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>56</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C28" s="2">
-        <v>-0.2</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>40</v>
+        <v>73</v>
+      </c>
+      <c r="B28" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28">
+        <v>0.02</v>
+      </c>
+      <c r="D28" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>56</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C29" s="2">
-        <v>0.18</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>41</v>
+        <v>73</v>
+      </c>
+      <c r="B29" t="s">
+        <v>78</v>
+      </c>
+      <c r="C29">
+        <v>0.7</v>
+      </c>
+      <c r="D29" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>56</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C30" s="2">
-        <v>-0.75</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>42</v>
+        <v>73</v>
+      </c>
+      <c r="B30" t="s">
+        <v>79</v>
+      </c>
+      <c r="C30">
+        <v>0.65</v>
+      </c>
+      <c r="D30" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="B31" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="C31">
-        <v>1.23</v>
+        <v>0.88</v>
       </c>
       <c r="D31" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="B32" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="C32">
-        <v>-0.77</v>
+        <v>1.03</v>
       </c>
       <c r="D32" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="B33" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="C33">
-        <v>-0.97</v>
+        <v>1.06</v>
       </c>
       <c r="D33" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>102</v>
+        <v>73</v>
       </c>
       <c r="B34" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D34" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>102</v>
+        <v>73</v>
       </c>
       <c r="B35" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="C35">
-        <v>0.02</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D35" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>102</v>
+        <v>73</v>
       </c>
       <c r="B36" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="C36">
-        <v>0.7</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D36" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>102</v>
+        <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="C37">
-        <v>0.65</v>
+        <v>-1.88</v>
       </c>
       <c r="D37" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>102</v>
+        <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="C38">
-        <v>0.88</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D38" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>102</v>
+        <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="C39">
-        <v>1.03</v>
+        <v>-0.24</v>
       </c>
       <c r="D39" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>102</v>
+        <v>37</v>
       </c>
       <c r="B40" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="C40">
-        <v>1.06</v>
+        <v>-1.77</v>
       </c>
       <c r="D40" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="B41" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="C41">
-        <v>1.1000000000000001</v>
+        <v>0</v>
       </c>
       <c r="D41" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="B42" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
       <c r="C42">
-        <v>1.1000000000000001</v>
+        <v>0.21</v>
       </c>
       <c r="D42" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="B43" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
       <c r="C43">
-        <v>1.1000000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="D43" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="B44" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="C44">
-        <v>-1.88</v>
+        <v>0.32</v>
       </c>
       <c r="D44" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="B45" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="C45">
-        <v>0.55000000000000004</v>
+        <v>0.38</v>
       </c>
       <c r="D45" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="B46" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="C46">
-        <v>-0.24</v>
+        <v>0.45</v>
       </c>
       <c r="D46" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="B47" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="C47">
-        <v>-1.77</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="D47" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>119</v>
+        <v>90</v>
       </c>
       <c r="B48" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="C48">
-        <v>0</v>
+        <v>0.65</v>
       </c>
       <c r="D48" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>119</v>
+        <v>90</v>
       </c>
       <c r="B49" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="C49">
-        <v>0.21</v>
+        <v>0.96</v>
       </c>
       <c r="D49" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>119</v>
+        <v>90</v>
       </c>
       <c r="B50" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="C50">
-        <v>0.27</v>
+        <v>1.07</v>
       </c>
       <c r="D50" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>119</v>
+        <v>54</v>
       </c>
       <c r="B51" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="C51">
-        <v>0.32</v>
+        <v>0.15</v>
       </c>
       <c r="D51" t="s">
-        <v>64</v>
+        <v>17</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>119</v>
+        <v>54</v>
       </c>
       <c r="B52" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
       <c r="C52">
-        <v>0.38</v>
+        <v>0.46</v>
       </c>
       <c r="D52" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>119</v>
+        <v>54</v>
       </c>
       <c r="B53" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
       <c r="C53">
-        <v>0.45</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="D53" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>119</v>
+        <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="C54">
-        <v>0.56000000000000005</v>
+        <v>-1.2</v>
       </c>
       <c r="D54" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>119</v>
+        <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
       <c r="C55">
-        <v>0.65</v>
+        <v>-0.3</v>
       </c>
       <c r="D55" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="B56" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
       <c r="C56">
-        <v>0.96</v>
+        <v>0</v>
       </c>
       <c r="D56" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="B57" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="C57">
-        <v>1.07</v>
+        <v>0.13</v>
       </c>
       <c r="D57" t="s">
-        <v>70</v>
+        <v>42</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>74</v>
+        <v>106</v>
       </c>
       <c r="B58" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="C58">
-        <v>0.15</v>
+        <v>0.23</v>
       </c>
       <c r="D58" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>74</v>
+        <v>106</v>
       </c>
       <c r="B59" t="s">
-        <v>131</v>
+        <v>110</v>
       </c>
       <c r="C59">
-        <v>0.46</v>
+        <v>0.24</v>
       </c>
       <c r="D59" t="s">
-        <v>71</v>
+        <v>44</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>74</v>
+        <v>106</v>
       </c>
       <c r="B60" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="C60">
-        <v>0.57999999999999996</v>
+        <v>0.23</v>
       </c>
       <c r="D60" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>74</v>
+        <v>106</v>
       </c>
       <c r="B61" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
       <c r="C61">
-        <v>-1.2</v>
+        <v>0.31</v>
       </c>
       <c r="D61" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>74</v>
+        <v>106</v>
       </c>
       <c r="B62" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
       <c r="C62">
-        <v>-0.3</v>
+        <v>0.26</v>
       </c>
       <c r="D62" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>135</v>
+        <v>106</v>
       </c>
       <c r="B63" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
       <c r="C63">
-        <v>0</v>
+        <v>0.21</v>
       </c>
       <c r="D63" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>135</v>
+        <v>106</v>
       </c>
       <c r="B64" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C64">
-        <v>0.13</v>
+        <v>0.4</v>
       </c>
       <c r="D64" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>135</v>
+        <v>106</v>
       </c>
       <c r="B65" t="s">
-        <v>138</v>
+        <v>116</v>
       </c>
       <c r="C65">
-        <v>0.23</v>
+        <v>0.6</v>
       </c>
       <c r="D65" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>135</v>
+        <v>56</v>
       </c>
       <c r="B66" t="s">
-        <v>139</v>
+        <v>117</v>
       </c>
       <c r="C66">
-        <v>0.24</v>
+        <v>-15.04</v>
       </c>
       <c r="D66" t="s">
-        <v>64</v>
+        <v>17</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>135</v>
+        <v>56</v>
       </c>
       <c r="B67" t="s">
-        <v>140</v>
+        <v>118</v>
       </c>
       <c r="C67">
-        <v>0.23</v>
+        <v>12.11</v>
       </c>
       <c r="D67" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>135</v>
+        <v>106</v>
       </c>
       <c r="B68" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
       <c r="C68">
         <v>0.31</v>
       </c>
       <c r="D68" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>135</v>
+        <v>106</v>
       </c>
       <c r="B69" t="s">
-        <v>142</v>
+        <v>113</v>
       </c>
       <c r="C69">
         <v>0.26</v>
       </c>
       <c r="D69" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>135</v>
+        <v>106</v>
       </c>
       <c r="B70" t="s">
-        <v>143</v>
+        <v>114</v>
       </c>
       <c r="C70">
         <v>0.21</v>
       </c>
       <c r="D70" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>135</v>
+        <v>106</v>
       </c>
       <c r="B71" t="s">
-        <v>144</v>
+        <v>115</v>
       </c>
       <c r="C71">
         <v>0.4</v>
       </c>
       <c r="D71" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>135</v>
+        <v>106</v>
       </c>
       <c r="B72" t="s">
-        <v>145</v>
+        <v>116</v>
       </c>
       <c r="C72">
         <v>0.6</v>
       </c>
       <c r="D72" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="B73" t="s">
-        <v>146</v>
+        <v>117</v>
       </c>
       <c r="C73">
         <v>-15.04</v>
       </c>
       <c r="D73" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="B74" t="s">
-        <v>147</v>
+        <v>118</v>
       </c>
       <c r="C74">
         <v>12.11</v>
       </c>
       <c r="D74" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New trip generation rates
</commit_message>
<xml_diff>
--- a/Parameter/FLUAM_ControlFile.xlsx
+++ b/Parameter/FLUAM_ControlFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Models\StateWide\TSM_Legacy\FLUAM\Parameter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F595D1E4-CD25-47FF-ACCA-F9A384B5E78B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C30C5321-0B8B-4468-AFA9-718049D62448}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0BE306DF-5F1F-4431-8911-019B31789681}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0BE306DF-5F1F-4431-8911-019B31789681}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="133">
   <si>
     <t>Value</t>
   </si>
@@ -480,18 +480,12 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -528,13 +522,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -853,7 +848,7 @@
   <dimension ref="A1:D74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -879,86 +874,86 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4">
         <v>0</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>1</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>1</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>6424</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>6461</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>100</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -984,7 +979,7 @@
         <v>119</v>
       </c>
       <c r="C9" s="2">
-        <v>565.88554648212198</v>
+        <v>0</v>
       </c>
       <c r="D9" t="s">
         <v>12</v>
@@ -997,8 +992,8 @@
       <c r="B10" t="s">
         <v>121</v>
       </c>
-      <c r="C10" s="3">
-        <v>10.809144997514515</v>
+      <c r="C10" s="5">
+        <v>0.75807058438147501</v>
       </c>
       <c r="D10" t="s">
         <v>13</v>
@@ -1011,8 +1006,8 @@
       <c r="B11" t="s">
         <v>122</v>
       </c>
-      <c r="C11" s="3">
-        <v>7.0701320225179662</v>
+      <c r="C11" s="5">
+        <v>0.85090168060698101</v>
       </c>
       <c r="D11" t="s">
         <v>14</v>
@@ -1025,50 +1020,50 @@
       <c r="B12" t="s">
         <v>123</v>
       </c>
-      <c r="C12" s="3">
-        <v>10.048530361121582</v>
+      <c r="C12" s="5">
+        <v>1.5472627674511401</v>
       </c>
       <c r="D12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="C13" s="2">
-        <v>4.2834951692240191</v>
+      <c r="C13" s="6">
+        <v>1.6350902224927799</v>
       </c>
       <c r="D13" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="C14" s="2">
-        <v>10.149223712027361</v>
+      <c r="C14" s="6">
+        <v>2.8035263259377698</v>
       </c>
       <c r="D14" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="C15" s="2">
-        <v>6.4854738028603665</v>
+      <c r="C15" s="6">
+        <v>1.9231837488047701</v>
       </c>
       <c r="D15" t="s">
         <v>131</v>
@@ -1082,7 +1077,7 @@
         <v>125</v>
       </c>
       <c r="C16" s="2">
-        <v>955.26841206494112</v>
+        <v>0</v>
       </c>
       <c r="D16" t="s">
         <v>16</v>

</xml_diff>